<commit_message>
updated codes 13,15,18 + outputs
updated codes :
13: added mean depth to groundwater
15: updated the selection model
18: updated plotting of simulation results to add distribution of gains.

Additionally, reran code 17.
All updated outputs committed.
</commit_message>
<xml_diff>
--- a/output/tables/simulation/simulation_results_7m.xlsx
+++ b/output/tables/simulation/simulation_results_7m.xlsx
@@ -1473,22 +1473,22 @@
         <v>8.51</v>
       </c>
       <c r="H26">
-        <v>7.41</v>
+        <v>7.36</v>
       </c>
       <c r="I26">
-        <v>87.11</v>
+        <v>86.51000000000001</v>
       </c>
       <c r="J26">
-        <v>161.56</v>
+        <v>155.12</v>
       </c>
       <c r="K26">
-        <v>193.55</v>
+        <v>195.12</v>
       </c>
       <c r="L26">
         <v>0</v>
       </c>
       <c r="M26">
-        <v>565.34</v>
+        <v>587.14</v>
       </c>
     </row>
     <row r="27">
@@ -1517,22 +1517,22 @@
         <v>8.51</v>
       </c>
       <c r="H27">
-        <v>7.41</v>
+        <v>7.36</v>
       </c>
       <c r="I27">
-        <v>87.11</v>
+        <v>86.51000000000001</v>
       </c>
       <c r="J27">
-        <v>161.56</v>
+        <v>155.12</v>
       </c>
       <c r="K27">
-        <v>193.55</v>
+        <v>195.12</v>
       </c>
       <c r="L27">
         <v>0</v>
       </c>
       <c r="M27">
-        <v>565.34</v>
+        <v>587.14</v>
       </c>
     </row>
     <row r="28">
@@ -1561,22 +1561,22 @@
         <v>8.52</v>
       </c>
       <c r="H28">
-        <v>7.41</v>
+        <v>7.36</v>
       </c>
       <c r="I28">
-        <v>86.98</v>
+        <v>86.38</v>
       </c>
       <c r="J28">
-        <v>161.49</v>
+        <v>155.1</v>
       </c>
       <c r="K28">
-        <v>193.52</v>
+        <v>195.09</v>
       </c>
       <c r="L28">
         <v>0</v>
       </c>
       <c r="M28">
-        <v>565.34</v>
+        <v>587.03</v>
       </c>
     </row>
     <row r="29">
@@ -1605,22 +1605,22 @@
         <v>23.63</v>
       </c>
       <c r="H29">
-        <v>20.06</v>
+        <v>19.95</v>
       </c>
       <c r="I29">
-        <v>84.92</v>
+        <v>84.43000000000001</v>
       </c>
       <c r="J29">
-        <v>144.72</v>
+        <v>143.97</v>
       </c>
       <c r="K29">
-        <v>191.56</v>
+        <v>193.19</v>
       </c>
       <c r="L29">
         <v>0</v>
       </c>
       <c r="M29">
-        <v>587.8099999999999</v>
+        <v>614.8</v>
       </c>
     </row>
     <row r="30">
@@ -1646,22 +1646,22 @@
         <v>8.52</v>
       </c>
       <c r="H30">
-        <v>7.41</v>
+        <v>7.36</v>
       </c>
       <c r="I30">
-        <v>86.98</v>
+        <v>86.38</v>
       </c>
       <c r="J30">
-        <v>161.49</v>
+        <v>155.1</v>
       </c>
       <c r="K30">
-        <v>193.52</v>
+        <v>195.09</v>
       </c>
       <c r="L30">
         <v>0</v>
       </c>
       <c r="M30">
-        <v>565.34</v>
+        <v>587.03</v>
       </c>
     </row>
     <row r="31">
@@ -1687,22 +1687,22 @@
         <v>23.63</v>
       </c>
       <c r="H31">
-        <v>20.06</v>
+        <v>19.95</v>
       </c>
       <c r="I31">
-        <v>84.92</v>
+        <v>84.43000000000001</v>
       </c>
       <c r="J31">
-        <v>144.72</v>
+        <v>143.97</v>
       </c>
       <c r="K31">
-        <v>191.56</v>
+        <v>193.18</v>
       </c>
       <c r="L31">
         <v>0</v>
       </c>
       <c r="M31">
-        <v>587.79</v>
+        <v>614.8</v>
       </c>
     </row>
     <row r="32">
@@ -1728,22 +1728,22 @@
         <v>23.79</v>
       </c>
       <c r="H32">
-        <v>20.1</v>
+        <v>19.98</v>
       </c>
       <c r="I32">
-        <v>84.48999999999999</v>
+        <v>84.01000000000001</v>
       </c>
       <c r="J32">
-        <v>144.72</v>
+        <v>143.97</v>
       </c>
       <c r="K32">
-        <v>191.5</v>
+        <v>193.14</v>
       </c>
       <c r="L32">
         <v>0</v>
       </c>
       <c r="M32">
-        <v>587.51</v>
+        <v>614.08</v>
       </c>
     </row>
     <row r="33">
@@ -1766,22 +1766,22 @@
         <v>23.79</v>
       </c>
       <c r="H33">
-        <v>20.1</v>
+        <v>19.99</v>
       </c>
       <c r="I33">
-        <v>84.5</v>
+        <v>84.01000000000001</v>
       </c>
       <c r="J33">
-        <v>144.72</v>
+        <v>143.97</v>
       </c>
       <c r="K33">
-        <v>191.5</v>
+        <v>193.14</v>
       </c>
       <c r="L33">
         <v>0</v>
       </c>
       <c r="M33">
-        <v>587.51</v>
+        <v>614.0599999999999</v>
       </c>
     </row>
     <row r="34">
@@ -1813,22 +1813,22 @@
         <v>8.51</v>
       </c>
       <c r="H34">
-        <v>5.74</v>
+        <v>5.81</v>
       </c>
       <c r="I34">
-        <v>67.43000000000001</v>
+        <v>68.34999999999999</v>
       </c>
       <c r="J34">
-        <v>167.96</v>
+        <v>157.58</v>
       </c>
       <c r="K34">
-        <v>203.48</v>
+        <v>197.52</v>
       </c>
       <c r="L34">
         <v>0</v>
       </c>
       <c r="M34">
-        <v>545.42</v>
+        <v>505.62</v>
       </c>
     </row>
     <row r="35">
@@ -1857,22 +1857,22 @@
         <v>8.51</v>
       </c>
       <c r="H35">
-        <v>5.74</v>
+        <v>5.81</v>
       </c>
       <c r="I35">
-        <v>67.43000000000001</v>
+        <v>68.34999999999999</v>
       </c>
       <c r="J35">
-        <v>167.96</v>
+        <v>157.58</v>
       </c>
       <c r="K35">
-        <v>203.48</v>
+        <v>197.52</v>
       </c>
       <c r="L35">
         <v>0</v>
       </c>
       <c r="M35">
-        <v>545.42</v>
+        <v>505.62</v>
       </c>
     </row>
     <row r="36">
@@ -1901,22 +1901,22 @@
         <v>8.52</v>
       </c>
       <c r="H36">
-        <v>5.74</v>
+        <v>5.81</v>
       </c>
       <c r="I36">
-        <v>67.28</v>
+        <v>68.2</v>
       </c>
       <c r="J36">
-        <v>167.96</v>
+        <v>157.58</v>
       </c>
       <c r="K36">
-        <v>203.48</v>
+        <v>197.52</v>
       </c>
       <c r="L36">
         <v>0</v>
       </c>
       <c r="M36">
-        <v>545.42</v>
+        <v>505.62</v>
       </c>
     </row>
     <row r="37">
@@ -1945,22 +1945,22 @@
         <v>23.63</v>
       </c>
       <c r="H37">
-        <v>12.39</v>
+        <v>12.55</v>
       </c>
       <c r="I37">
-        <v>52.43</v>
+        <v>53.1</v>
       </c>
       <c r="J37">
-        <v>166.42</v>
+        <v>157.58</v>
       </c>
       <c r="K37">
-        <v>211.62</v>
+        <v>204.87</v>
       </c>
       <c r="L37">
         <v>0</v>
       </c>
       <c r="M37">
-        <v>590</v>
+        <v>577.77</v>
       </c>
     </row>
     <row r="38">
@@ -1986,22 +1986,22 @@
         <v>8.52</v>
       </c>
       <c r="H38">
-        <v>5.74</v>
+        <v>5.81</v>
       </c>
       <c r="I38">
-        <v>67.28</v>
+        <v>68.2</v>
       </c>
       <c r="J38">
-        <v>167.96</v>
+        <v>157.58</v>
       </c>
       <c r="K38">
-        <v>203.48</v>
+        <v>197.52</v>
       </c>
       <c r="L38">
         <v>0</v>
       </c>
       <c r="M38">
-        <v>545.42</v>
+        <v>505.62</v>
       </c>
     </row>
     <row r="39">
@@ -2027,22 +2027,22 @@
         <v>23.63</v>
       </c>
       <c r="H39">
-        <v>12.39</v>
+        <v>12.55</v>
       </c>
       <c r="I39">
-        <v>52.43</v>
+        <v>53.1</v>
       </c>
       <c r="J39">
-        <v>166.42</v>
+        <v>157.58</v>
       </c>
       <c r="K39">
-        <v>211.62</v>
+        <v>204.87</v>
       </c>
       <c r="L39">
         <v>0</v>
       </c>
       <c r="M39">
-        <v>590</v>
+        <v>577.77</v>
       </c>
     </row>
     <row r="40">
@@ -2068,22 +2068,22 @@
         <v>23.79</v>
       </c>
       <c r="H40">
-        <v>12.39</v>
+        <v>12.55</v>
       </c>
       <c r="I40">
-        <v>52.07</v>
+        <v>52.74</v>
       </c>
       <c r="J40">
-        <v>166.42</v>
+        <v>157.58</v>
       </c>
       <c r="K40">
-        <v>211.62</v>
+        <v>204.87</v>
       </c>
       <c r="L40">
         <v>0</v>
       </c>
       <c r="M40">
-        <v>590</v>
+        <v>577.77</v>
       </c>
     </row>
     <row r="41">
@@ -2106,22 +2106,22 @@
         <v>23.79</v>
       </c>
       <c r="H41">
-        <v>12.39</v>
+        <v>12.55</v>
       </c>
       <c r="I41">
-        <v>52.07</v>
+        <v>52.73</v>
       </c>
       <c r="J41">
-        <v>166.42</v>
+        <v>157.58</v>
       </c>
       <c r="K41">
-        <v>211.62</v>
+        <v>204.87</v>
       </c>
       <c r="L41">
         <v>0</v>
       </c>
       <c r="M41">
-        <v>590</v>
+        <v>577.77</v>
       </c>
     </row>
     <row r="42">
@@ -2159,16 +2159,16 @@
         <v>29.55</v>
       </c>
       <c r="J42">
-        <v>226.07</v>
+        <v>216.63</v>
       </c>
       <c r="K42">
-        <v>240.83</v>
+        <v>234.58</v>
       </c>
       <c r="L42">
         <v>0</v>
       </c>
       <c r="M42">
-        <v>594.5</v>
+        <v>597.8</v>
       </c>
     </row>
     <row r="43">
@@ -2203,16 +2203,16 @@
         <v>29.55</v>
       </c>
       <c r="J43">
-        <v>226.07</v>
+        <v>216.63</v>
       </c>
       <c r="K43">
-        <v>240.83</v>
+        <v>234.58</v>
       </c>
       <c r="L43">
         <v>0</v>
       </c>
       <c r="M43">
-        <v>594.5</v>
+        <v>597.8</v>
       </c>
     </row>
     <row r="44">
@@ -2247,16 +2247,16 @@
         <v>29.52</v>
       </c>
       <c r="J44">
-        <v>225.68</v>
+        <v>216.1</v>
       </c>
       <c r="K44">
-        <v>240.58</v>
+        <v>234.33</v>
       </c>
       <c r="L44">
         <v>0</v>
       </c>
       <c r="M44">
-        <v>594.5</v>
+        <v>597.71</v>
       </c>
     </row>
     <row r="45">
@@ -2291,16 +2291,16 @@
         <v>23.04</v>
       </c>
       <c r="J45">
-        <v>167.43</v>
+        <v>162.75</v>
       </c>
       <c r="K45">
-        <v>223.29</v>
+        <v>218.01</v>
       </c>
       <c r="L45">
         <v>0</v>
       </c>
       <c r="M45">
-        <v>600.8200000000001</v>
+        <v>605.87</v>
       </c>
     </row>
     <row r="46">
@@ -2332,16 +2332,16 @@
         <v>29.52</v>
       </c>
       <c r="J46">
-        <v>225.68</v>
+        <v>216.1</v>
       </c>
       <c r="K46">
-        <v>240.58</v>
+        <v>234.33</v>
       </c>
       <c r="L46">
         <v>0</v>
       </c>
       <c r="M46">
-        <v>594.5</v>
+        <v>597.71</v>
       </c>
     </row>
     <row r="47">
@@ -2373,16 +2373,16 @@
         <v>23.04</v>
       </c>
       <c r="J47">
-        <v>167.4</v>
+        <v>162.57</v>
       </c>
       <c r="K47">
-        <v>223.27</v>
+        <v>217.99</v>
       </c>
       <c r="L47">
         <v>0</v>
       </c>
       <c r="M47">
-        <v>600.8200000000001</v>
+        <v>605.87</v>
       </c>
     </row>
     <row r="48">
@@ -2414,16 +2414,16 @@
         <v>22.95</v>
       </c>
       <c r="J48">
-        <v>166.07</v>
+        <v>161.21</v>
       </c>
       <c r="K48">
-        <v>222.73</v>
+        <v>217.47</v>
       </c>
       <c r="L48">
         <v>0</v>
       </c>
       <c r="M48">
-        <v>600.6900000000001</v>
+        <v>605.6</v>
       </c>
     </row>
     <row r="49">
@@ -2452,16 +2452,16 @@
         <v>22.95</v>
       </c>
       <c r="J49">
-        <v>166.05</v>
+        <v>161.07</v>
       </c>
       <c r="K49">
-        <v>222.71</v>
+        <v>217.45</v>
       </c>
       <c r="L49">
         <v>0</v>
       </c>
       <c r="M49">
-        <v>600.67</v>
+        <v>605.5700000000001</v>
       </c>
     </row>
     <row r="50">
@@ -3513,22 +3513,22 @@
         <v>8.51</v>
       </c>
       <c r="H74">
-        <v>7.76</v>
+        <v>7.72</v>
       </c>
       <c r="I74">
-        <v>91.23</v>
+        <v>90.7</v>
       </c>
       <c r="J74">
-        <v>184.88</v>
+        <v>173.8</v>
       </c>
       <c r="K74">
-        <v>221.8</v>
+        <v>224.08</v>
       </c>
       <c r="L74">
         <v>0</v>
       </c>
       <c r="M74">
-        <v>634.37</v>
+        <v>657.92</v>
       </c>
     </row>
     <row r="75">
@@ -3557,22 +3557,22 @@
         <v>8.51</v>
       </c>
       <c r="H75">
-        <v>7.76</v>
+        <v>7.72</v>
       </c>
       <c r="I75">
-        <v>91.23</v>
+        <v>90.7</v>
       </c>
       <c r="J75">
-        <v>184.88</v>
+        <v>173.8</v>
       </c>
       <c r="K75">
-        <v>221.8</v>
+        <v>224.08</v>
       </c>
       <c r="L75">
         <v>0</v>
       </c>
       <c r="M75">
-        <v>634.37</v>
+        <v>657.92</v>
       </c>
     </row>
     <row r="76">
@@ -3601,22 +3601,22 @@
         <v>8.52</v>
       </c>
       <c r="H76">
-        <v>7.76</v>
+        <v>7.72</v>
       </c>
       <c r="I76">
-        <v>91.09</v>
+        <v>90.56</v>
       </c>
       <c r="J76">
-        <v>184.9</v>
+        <v>173.82</v>
       </c>
       <c r="K76">
-        <v>221.8</v>
+        <v>224.09</v>
       </c>
       <c r="L76">
         <v>0</v>
       </c>
       <c r="M76">
-        <v>634.37</v>
+        <v>657.4</v>
       </c>
     </row>
     <row r="77">
@@ -3645,22 +3645,22 @@
         <v>23.63</v>
       </c>
       <c r="H77">
-        <v>21.44</v>
+        <v>21.34</v>
       </c>
       <c r="I77">
-        <v>90.77</v>
+        <v>90.34999999999999</v>
       </c>
       <c r="J77">
-        <v>190.7</v>
+        <v>182.21</v>
       </c>
       <c r="K77">
-        <v>257.11</v>
+        <v>260.68</v>
       </c>
       <c r="L77">
         <v>0</v>
       </c>
       <c r="M77">
-        <v>723.54</v>
+        <v>749.5599999999999</v>
       </c>
     </row>
     <row r="78">
@@ -3686,22 +3686,22 @@
         <v>8.52</v>
       </c>
       <c r="H78">
-        <v>7.76</v>
+        <v>7.72</v>
       </c>
       <c r="I78">
-        <v>91.09</v>
+        <v>90.56</v>
       </c>
       <c r="J78">
-        <v>184.9</v>
+        <v>173.82</v>
       </c>
       <c r="K78">
-        <v>221.8</v>
+        <v>224.09</v>
       </c>
       <c r="L78">
         <v>0</v>
       </c>
       <c r="M78">
-        <v>634.37</v>
+        <v>657.4</v>
       </c>
     </row>
     <row r="79">
@@ -3727,22 +3727,22 @@
         <v>23.63</v>
       </c>
       <c r="H79">
-        <v>21.45</v>
+        <v>21.35</v>
       </c>
       <c r="I79">
-        <v>90.77</v>
+        <v>90.34999999999999</v>
       </c>
       <c r="J79">
-        <v>190.7</v>
+        <v>182.21</v>
       </c>
       <c r="K79">
-        <v>257.11</v>
+        <v>260.67</v>
       </c>
       <c r="L79">
         <v>0</v>
       </c>
       <c r="M79">
-        <v>723.5</v>
+        <v>749.54</v>
       </c>
     </row>
     <row r="80">
@@ -3768,22 +3768,22 @@
         <v>23.79</v>
       </c>
       <c r="H80">
-        <v>21.48</v>
+        <v>21.38</v>
       </c>
       <c r="I80">
-        <v>90.3</v>
+        <v>89.88</v>
       </c>
       <c r="J80">
-        <v>190.78</v>
+        <v>182.3</v>
       </c>
       <c r="K80">
-        <v>257.1</v>
+        <v>260.67</v>
       </c>
       <c r="L80">
         <v>0</v>
       </c>
       <c r="M80">
-        <v>723.09</v>
+        <v>749.39</v>
       </c>
     </row>
     <row r="81">
@@ -3806,22 +3806,22 @@
         <v>23.79</v>
       </c>
       <c r="H81">
-        <v>21.48</v>
+        <v>21.38</v>
       </c>
       <c r="I81">
-        <v>90.3</v>
+        <v>89.88</v>
       </c>
       <c r="J81">
-        <v>190.78</v>
+        <v>182.29</v>
       </c>
       <c r="K81">
-        <v>257.1</v>
+        <v>260.67</v>
       </c>
       <c r="L81">
         <v>0</v>
       </c>
       <c r="M81">
-        <v>723.08</v>
+        <v>749.38</v>
       </c>
     </row>
     <row r="82">
@@ -3853,22 +3853,22 @@
         <v>8.51</v>
       </c>
       <c r="H82">
-        <v>6</v>
+        <v>6.08</v>
       </c>
       <c r="I82">
-        <v>70.52</v>
+        <v>71.44</v>
       </c>
       <c r="J82">
-        <v>193.59</v>
+        <v>177.55</v>
       </c>
       <c r="K82">
-        <v>229.12</v>
+        <v>222.66</v>
       </c>
       <c r="L82">
         <v>0</v>
       </c>
       <c r="M82">
-        <v>577.54</v>
+        <v>545.48</v>
       </c>
     </row>
     <row r="83">
@@ -3897,22 +3897,22 @@
         <v>8.51</v>
       </c>
       <c r="H83">
-        <v>6</v>
+        <v>6.08</v>
       </c>
       <c r="I83">
-        <v>70.52</v>
+        <v>71.44</v>
       </c>
       <c r="J83">
-        <v>193.59</v>
+        <v>177.55</v>
       </c>
       <c r="K83">
-        <v>229.12</v>
+        <v>222.66</v>
       </c>
       <c r="L83">
         <v>0</v>
       </c>
       <c r="M83">
-        <v>577.54</v>
+        <v>545.48</v>
       </c>
     </row>
     <row r="84">
@@ -3941,22 +3941,22 @@
         <v>8.52</v>
       </c>
       <c r="H84">
-        <v>6</v>
+        <v>6.08</v>
       </c>
       <c r="I84">
-        <v>70.37</v>
+        <v>71.29000000000001</v>
       </c>
       <c r="J84">
-        <v>193.59</v>
+        <v>177.55</v>
       </c>
       <c r="K84">
-        <v>229.12</v>
+        <v>222.66</v>
       </c>
       <c r="L84">
         <v>0</v>
       </c>
       <c r="M84">
-        <v>577.54</v>
+        <v>545.48</v>
       </c>
     </row>
     <row r="85">
@@ -3985,22 +3985,22 @@
         <v>23.63</v>
       </c>
       <c r="H85">
-        <v>13.01</v>
+        <v>13.17</v>
       </c>
       <c r="I85">
-        <v>55.07</v>
+        <v>55.76</v>
       </c>
       <c r="J85">
-        <v>199.43</v>
+        <v>185.61</v>
       </c>
       <c r="K85">
-        <v>257.28</v>
+        <v>249.19</v>
       </c>
       <c r="L85">
         <v>0</v>
       </c>
       <c r="M85">
-        <v>774.53</v>
+        <v>747.66</v>
       </c>
     </row>
     <row r="86">
@@ -4026,22 +4026,22 @@
         <v>8.52</v>
       </c>
       <c r="H86">
-        <v>6</v>
+        <v>6.08</v>
       </c>
       <c r="I86">
-        <v>70.37</v>
+        <v>71.29000000000001</v>
       </c>
       <c r="J86">
-        <v>193.59</v>
+        <v>177.55</v>
       </c>
       <c r="K86">
-        <v>229.12</v>
+        <v>222.66</v>
       </c>
       <c r="L86">
         <v>0</v>
       </c>
       <c r="M86">
-        <v>577.54</v>
+        <v>545.48</v>
       </c>
     </row>
     <row r="87">
@@ -4067,22 +4067,22 @@
         <v>23.63</v>
       </c>
       <c r="H87">
-        <v>13.01</v>
+        <v>13.17</v>
       </c>
       <c r="I87">
-        <v>55.07</v>
+        <v>55.76</v>
       </c>
       <c r="J87">
-        <v>199.43</v>
+        <v>185.61</v>
       </c>
       <c r="K87">
-        <v>257.28</v>
+        <v>249.19</v>
       </c>
       <c r="L87">
         <v>0</v>
       </c>
       <c r="M87">
-        <v>774.53</v>
+        <v>747.66</v>
       </c>
     </row>
     <row r="88">
@@ -4108,22 +4108,22 @@
         <v>23.79</v>
       </c>
       <c r="H88">
-        <v>13.01</v>
+        <v>13.17</v>
       </c>
       <c r="I88">
-        <v>54.7</v>
+        <v>55.38</v>
       </c>
       <c r="J88">
-        <v>199.43</v>
+        <v>185.61</v>
       </c>
       <c r="K88">
-        <v>257.28</v>
+        <v>249.19</v>
       </c>
       <c r="L88">
         <v>0</v>
       </c>
       <c r="M88">
-        <v>774.53</v>
+        <v>747.66</v>
       </c>
     </row>
     <row r="89">
@@ -4146,22 +4146,22 @@
         <v>23.79</v>
       </c>
       <c r="H89">
-        <v>13.01</v>
+        <v>13.17</v>
       </c>
       <c r="I89">
-        <v>54.69</v>
+        <v>55.38</v>
       </c>
       <c r="J89">
-        <v>199.43</v>
+        <v>185.61</v>
       </c>
       <c r="K89">
-        <v>257.28</v>
+        <v>249.19</v>
       </c>
       <c r="L89">
         <v>0</v>
       </c>
       <c r="M89">
-        <v>774.53</v>
+        <v>747.66</v>
       </c>
     </row>
     <row r="90">
@@ -4199,16 +4199,16 @@
         <v>28.06</v>
       </c>
       <c r="J90">
-        <v>240.17</v>
+        <v>229.68</v>
       </c>
       <c r="K90">
-        <v>251.62</v>
+        <v>245.63</v>
       </c>
       <c r="L90">
         <v>0</v>
       </c>
       <c r="M90">
-        <v>604.36</v>
+        <v>607.5700000000001</v>
       </c>
     </row>
     <row r="91">
@@ -4243,16 +4243,16 @@
         <v>28.06</v>
       </c>
       <c r="J91">
-        <v>240.17</v>
+        <v>229.68</v>
       </c>
       <c r="K91">
-        <v>251.62</v>
+        <v>245.63</v>
       </c>
       <c r="L91">
         <v>0</v>
       </c>
       <c r="M91">
-        <v>604.36</v>
+        <v>607.5700000000001</v>
       </c>
     </row>
     <row r="92">
@@ -4287,16 +4287,16 @@
         <v>28.03</v>
       </c>
       <c r="J92">
-        <v>240.12</v>
+        <v>229.66</v>
       </c>
       <c r="K92">
-        <v>251.54</v>
+        <v>245.55</v>
       </c>
       <c r="L92">
         <v>0</v>
       </c>
       <c r="M92">
-        <v>604.12</v>
+        <v>607.5700000000001</v>
       </c>
     </row>
     <row r="93">
@@ -4331,16 +4331,16 @@
         <v>22.48</v>
       </c>
       <c r="J93">
-        <v>213.99</v>
+        <v>205.98</v>
       </c>
       <c r="K93">
-        <v>247.62</v>
+        <v>242.36</v>
       </c>
       <c r="L93">
         <v>0</v>
       </c>
       <c r="M93">
-        <v>635.7</v>
+        <v>640.34</v>
       </c>
     </row>
     <row r="94">
@@ -4372,16 +4372,16 @@
         <v>28.03</v>
       </c>
       <c r="J94">
-        <v>240.12</v>
+        <v>229.66</v>
       </c>
       <c r="K94">
-        <v>251.54</v>
+        <v>245.55</v>
       </c>
       <c r="L94">
         <v>0</v>
       </c>
       <c r="M94">
-        <v>604.12</v>
+        <v>607.5700000000001</v>
       </c>
     </row>
     <row r="95">
@@ -4413,16 +4413,16 @@
         <v>22.48</v>
       </c>
       <c r="J95">
-        <v>213.91</v>
+        <v>205.9</v>
       </c>
       <c r="K95">
-        <v>247.59</v>
+        <v>242.33</v>
       </c>
       <c r="L95">
         <v>0</v>
       </c>
       <c r="M95">
-        <v>635.6900000000001</v>
+        <v>640.3200000000001</v>
       </c>
     </row>
     <row r="96">
@@ -4454,16 +4454,16 @@
         <v>22.39</v>
       </c>
       <c r="J96">
-        <v>213.87</v>
+        <v>205.78</v>
       </c>
       <c r="K96">
-        <v>247.55</v>
+        <v>242.31</v>
       </c>
       <c r="L96">
         <v>0</v>
       </c>
       <c r="M96">
-        <v>635.65</v>
+        <v>640.24</v>
       </c>
     </row>
     <row r="97">
@@ -4492,16 +4492,16 @@
         <v>22.39</v>
       </c>
       <c r="J97">
-        <v>213.86</v>
+        <v>205.75</v>
       </c>
       <c r="K97">
-        <v>247.52</v>
+        <v>242.28</v>
       </c>
       <c r="L97">
         <v>0</v>
       </c>
       <c r="M97">
-        <v>635.63</v>
+        <v>640.22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>